<commit_message>
Update Kho gửi phòng sxbh 10_2025.xlsx
</commit_message>
<xml_diff>
--- a/5.Other/Thiết bị kho gửi/2025/Kho gửi phòng sxbh 10_2025.xlsx
+++ b/5.Other/Thiết bị kho gửi/2025/Kho gửi phòng sxbh 10_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VNET\5.Other\Thiết bị kho gửi\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D4541A-CFCE-4821-9F71-C9EACFB75B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC1F5A9-7470-406D-8017-ABC8CBE0EE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6780" yWindow="2235" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nhập xuất tồn" sheetId="1" r:id="rId1"/>
@@ -509,7 +509,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,18 +595,18 @@
       </c>
       <c r="E5" s="3">
         <f>Xuất!AH6+'Hủy tb'!AH6</f>
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" ref="F5:F6" si="0">C5+D5-E5</f>
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
       </c>
       <c r="H5" s="1">
         <f>F5-G5</f>
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1757,7 +1757,7 @@
   <dimension ref="A1:AH19"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2009,7 +2009,9 @@
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="7"/>
+      <c r="J6" s="7">
+        <v>9</v>
+      </c>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
@@ -2035,7 +2037,7 @@
       <c r="AG6" s="8"/>
       <c r="AH6" s="8">
         <f t="shared" ref="AH6:AH19" si="0">SUM(C6:AG6)</f>
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">

</xml_diff>